<commit_message>
Attribute und constraints in xlsx beschrieben
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -13,19 +13,20 @@
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
-    <sheet name="AssetKindItem" sheetId="2" r:id="rId2"/>
-    <sheet name="ManCatLabelItem" sheetId="3" r:id="rId3"/>
-    <sheet name="AssetFormatItem" sheetId="4" r:id="rId4"/>
-    <sheet name="ContactKindItem" sheetId="5" r:id="rId5"/>
-    <sheet name="LanguageItem" sheetId="6" r:id="rId6"/>
-    <sheet name="GeomQualityItem" sheetId="7" r:id="rId7"/>
-    <sheet name="AutoCatLabelItem" sheetId="8" r:id="rId8"/>
-    <sheet name="AutoObjectCatItem" sheetId="9" r:id="rId9"/>
-    <sheet name="NatRelItem" sheetId="10" r:id="rId10"/>
-    <sheet name="PubChannelItem" sheetId="11" r:id="rId11"/>
-    <sheet name="StatusWorkItem" sheetId="12" r:id="rId12"/>
-    <sheet name="LegalDocItem" sheetId="13" r:id="rId13"/>
-    <sheet name="StatusAssetUseItem" sheetId="14" r:id="rId14"/>
+    <sheet name="Constraints" sheetId="15" r:id="rId2"/>
+    <sheet name="AssetKindItem" sheetId="2" r:id="rId3"/>
+    <sheet name="ManCatLabelItem" sheetId="3" r:id="rId4"/>
+    <sheet name="AssetFormatItem" sheetId="4" r:id="rId5"/>
+    <sheet name="ContactKindItem" sheetId="5" r:id="rId6"/>
+    <sheet name="LanguageItem" sheetId="6" r:id="rId7"/>
+    <sheet name="GeomQualityItem" sheetId="7" r:id="rId8"/>
+    <sheet name="AutoCatLabelItem" sheetId="8" r:id="rId9"/>
+    <sheet name="AutoObjectCatItem" sheetId="9" r:id="rId10"/>
+    <sheet name="NatRelItem" sheetId="10" r:id="rId11"/>
+    <sheet name="PubChannelItem" sheetId="11" r:id="rId12"/>
+    <sheet name="StatusWorkItem" sheetId="12" r:id="rId13"/>
+    <sheet name="LegalDocItem" sheetId="13" r:id="rId14"/>
+    <sheet name="StatusAssetUseItem" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="674">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -1839,27 +1840,15 @@
     <t>401b1f46-3a45-4c19-a738-b03db948d224</t>
   </si>
   <si>
-    <t xml:space="preserve">  /** Wenn Kind == report, dann muss TitlePublic gesetzt sein.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  */</t>
   </si>
   <si>
-    <t xml:space="preserve">   SET CONSTRAINT WHERE Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "report": </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   DEFINED (TitlePublic);</t>
-  </si>
-  <si>
     <t xml:space="preserve">  /** Wenn IsExtract gesetzt (es handelt sich dann um ein extrahiertes Objekt, z.B. Bohrprofil aus einem Bericht), dann darf Kind nicht "report" oder "package" sein. Sonst darf IsExtract nicht gesetzt sein.</t>
   </si>
   <si>
     <t xml:space="preserve">  SET CONSTRAINT WHERE IsExtract: </t>
   </si>
   <si>
-    <t xml:space="preserve">  NOT (Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package") AND </t>
-  </si>
-  <si>
     <t xml:space="preserve">  NOT (Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "report");</t>
   </si>
   <si>
@@ -1909,45 +1898,6 @@
   </si>
   <si>
     <t xml:space="preserve">  AssetItemMain-&gt;Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package";</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  SET CONSTRAINT WHERE NOT (InternalUse-&gt;IsAvailable):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     NOT (PublicUse-&gt;IsAvailable);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  /** Wenn das Startdatum der Öffentichennutzung gesetzt ist, dann muss auch das Startdatum der Internennutzung gesetzt sein und das interne Startdatum muss kleiner oder gleich dem öffentlichen sein.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  SET CONSTRAINT WHERE DEFINED (PublicUse-&gt;DateStartAvailability): </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  DEFINED(InternalUse-&gt;DateStartAvailability) AND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (InternalUse-&gt;DateStartAvailability &lt;= PublicUse-&gt;DateStartAvailability);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  /** Wenn das öffentliche Startdatum gesetzt ist, dann darf der öffentliche Nutzungsstatus nicht auf TRUE (= nutzbar) stehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  SET CONSTRAINT WHERE DEFINED (PublicUse-&gt;DateStartAvailability):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  NOT (PublicUse-&gt;IsAvailable);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  /** Wenn das interne Startdatum gesetzt ist, dann darf der interne Nutzungsstatus nicht auf TRUE (= nutzbar) stehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  SET CONSTRAINT WHERE DEFINED (InternalUse-&gt;DateStartAvailability):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  NOT (InternalUse-&gt;IsAvailable);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  /** Wenn IsInternalUse == False, dann muss IsPublicUse auch == False sein.</t>
   </si>
   <si>
     <r>
@@ -1992,25 +1942,162 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CONSTRAINTS: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Klasse LGAssetItem</t>
-    </r>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Wenn Kind == report, dann muss TitlePublic gesetzt sein</t>
+  </si>
+  <si>
+    <t>AssetItem</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "report": DEFINED (TitlePublic);</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE IsExtract: NOT (Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package") AND NOT (Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "report");</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package": Format-&gt;Reference-&gt;Name-&gt; LocalisedText-&gt;Text == "zip";</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE Format-&gt;Reference-&gt;Name-&gt; LocalisedText-&gt;Text == "zip": Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package";</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE DEFINED (FormatComposition): Format-&gt;Reference-&gt;Name-&gt; LocalisedText-&gt;Text == "zip";</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE Format-&gt;Reference-&gt;Name-&gt; LocalisedText-&gt;Text == "zip": DEFINED (FormatComposition);</t>
+  </si>
+  <si>
+    <t>Element name</t>
+  </si>
+  <si>
+    <t>Element type</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>association</t>
+  </si>
+  <si>
+    <t>AssetItemMain_AssetItemPart</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE AssetItemPart-&gt;IsExtract: NOT(AssetItemMain-&gt;IsExtract) AND NOT(AssetItemMain-&gt;Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package");</t>
+  </si>
+  <si>
+    <t>MANDATORY CONSTRAINT NOT(AssetItemPart-&gt;Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET CONSTRAINT WHERE NOT( AssetItemPart-&gt;IsExtract): AssetItemMain-&gt;Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package";
+</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Wenn das AssetPart ein Extrakt ist, muss das übergeordnete AssetMain das Kind == "report" haben oder es darf kein Extrakt sein und das übergeordnete AssetMain ist ein "package"</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE AssetItemPart-&gt;IsExtract: AssetItemMain-&gt;Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text =="report";</t>
+  </si>
+  <si>
+    <t>Wenn AssetItemPart-&gt;IsExtract == True, dann muss Kind == "package" sein</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE NOT( AssetItemPart-&gt;IsExtract): AssetItemMain-&gt;Kind-&gt;Reference-&gt;Name-&gt;LocalisedText-&gt;Text == "package";</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>replaced</t>
+  </si>
+  <si>
+    <t>#ref</t>
+  </si>
+  <si>
+    <t>Wenn "IsExtract" gesetzt (es handelt sich dann um ein extrahiertes Objekt, z.B. Bohrprofil aus einem Bericht), dann darf "Kind" nicht "report" oder "package" sein. Sonst darf IsExtract nicht gesetzt sein.</t>
+  </si>
+  <si>
+    <t>Wenn "Kind" == "package", dann muss "Format" == "Archiv (zip)" sein</t>
+  </si>
+  <si>
+    <t>Wenn "Format" == "Archiv (zip)", dann muss "Kind" == "package" sein</t>
+  </si>
+  <si>
+    <t>"FormatComposition" darf nur ausgefüllt sein, wenn für das "Format" "zip" gewählt wurde</t>
+  </si>
+  <si>
+    <t>Wenn "FormatComposition" ausgefüllt ist, muss für das "Format" "zip" gewählt werden</t>
+  </si>
+  <si>
+    <t>deleted, weil constraint nicht erforderlich. Neu TitleOriginal "MANDATORY" und "TitlePublic" optional. Der Erfasser muss entscheiden, ob der Originaltitel sensible Daten enthält</t>
+  </si>
+  <si>
+    <t>replaced, weil constraint nur mit #7 funktioniert</t>
+  </si>
+  <si>
+    <t>replaced, weil constraint fachlich nicht korrekt. Es düfen alle Kinds Extracts enthalten</t>
+  </si>
+  <si>
+    <t>Ein "AssetPart" darf nur ein "Extract" sein, wenn das zugehörige "AssetMain" selber kein "Extract" ist und es selber (das "AssetMain") nicht vom "Kind" == "package" ist
+Ein Package darf kein Extract enhalten</t>
+  </si>
+  <si>
+    <t>Wenn ein "AssetPart" kein "Extract" ist, dann muss das zugehörige "AssetMain" ein "Kind" == "package" sein</t>
+  </si>
+  <si>
+    <t>Ein "AssetPart" darf selber nicht vom "Kind" == "package" sein</t>
+  </si>
+  <si>
+    <t>9, 10, 11</t>
+  </si>
+  <si>
+    <t>LG_GeoAssets_V2</t>
+  </si>
+  <si>
+    <t>Wenn IsInternalUse == False, dann muss IsPublicUse auch == False sein</t>
+  </si>
+  <si>
+    <t>LGAssetItem</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE NOT (InternalUse-&gt;IsAvailable): NOT (PublicUse-&gt;IsAvailable);</t>
+  </si>
+  <si>
+    <t>Wenn das Startdatum der Öffentichennutzung gesetzt ist, dann muss auch das Startdatum der Internennutzung gesetzt sein und das interne Startdatum muss kleiner oder gleich dem öffentlichen sein</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE DEFINED (PublicUse-&gt;DateStartAvailability): DEFINED(InternalUse-&gt;DateStartAvailability) AND (InternalUse-&gt;DateStartAvailability &lt;= PublicUse-&gt;DateStartAvailability);</t>
+  </si>
+  <si>
+    <t>Wenn das öffentliche Startdatum gesetzt ist, dann darf der öffentliche Nutzungsstatus nicht auf TRUE (= nutzbar) stehen</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE DEFINED (PublicUse-&gt;DateStartAvailability): NOT (PublicUse-&gt;IsAvailable);</t>
+  </si>
+  <si>
+    <t>Wenn das interne Startdatum gesetzt ist, dann darf der interne Nutzungsstatus nicht auf TRUE (= nutzbar) stehen</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE DEFINED (InternalUse-&gt;DateStartAvailability): NOT (InternalUse-&gt;IsAvailable);</t>
   </si>
 </sst>
 </file>
@@ -2085,14 +2172,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2111,6 +2197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2125,7 +2217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2158,6 +2250,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2200,7 +2310,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="5982337" y="208101"/>
-          <a:ext cx="11162429" cy="10185318"/>
+          <a:ext cx="11162429" cy="9994818"/>
           <a:chOff x="5979863" y="206451"/>
           <a:chExt cx="11162429" cy="9516507"/>
         </a:xfrm>
@@ -2607,10 +2717,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A2:U60"/>
+  <dimension ref="A2:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="U43" sqref="U43:U60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2620,32 +2730,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U2" s="11" t="s">
-        <v>637</v>
-      </c>
+      <c r="U2" s="11"/>
     </row>
     <row r="3" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U3" s="11" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="39" x14ac:dyDescent="0.35">
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:21" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U4" s="11" t="s">
-        <v>601</v>
-      </c>
+      <c r="U4" s="11"/>
     </row>
     <row r="5" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U5" s="11" t="s">
-        <v>602</v>
-      </c>
+      <c r="U5" s="11"/>
     </row>
     <row r="6" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U6" s="11" t="s">
-        <v>603</v>
-      </c>
+      <c r="U6" s="11"/>
     </row>
     <row r="7" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
@@ -2657,9 +2757,7 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="11" t="s">
-        <v>604</v>
-      </c>
+      <c r="U7" s="11"/>
     </row>
     <row r="8" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
@@ -2671,116 +2769,76 @@
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="U8" s="11" t="s">
-        <v>601</v>
-      </c>
+      <c r="U8" s="11"/>
     </row>
     <row r="9" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U9" s="11" t="s">
-        <v>605</v>
-      </c>
+      <c r="U9" s="11"/>
     </row>
     <row r="10" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U10" s="11" t="s">
-        <v>606</v>
-      </c>
+      <c r="U10" s="11"/>
     </row>
     <row r="11" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U11" s="11" t="s">
-        <v>607</v>
-      </c>
+      <c r="U11" s="11"/>
     </row>
     <row r="12" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U12" s="11" t="s">
-        <v>608</v>
-      </c>
+      <c r="U12" s="11"/>
     </row>
     <row r="13" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U13" s="11" t="s">
-        <v>601</v>
-      </c>
+      <c r="U13" s="11"/>
     </row>
     <row r="14" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U14" s="11" t="s">
-        <v>609</v>
-      </c>
+      <c r="U14" s="11"/>
     </row>
     <row r="15" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U15" s="11" t="s">
-        <v>610</v>
-      </c>
+      <c r="U15" s="11"/>
     </row>
     <row r="16" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U16" s="11" t="s">
-        <v>611</v>
-      </c>
+      <c r="U16" s="11"/>
     </row>
     <row r="17" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U17" s="11" t="s">
-        <v>601</v>
-      </c>
+      <c r="U17" s="11"/>
     </row>
     <row r="18" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U18" s="11" t="s">
-        <v>612</v>
-      </c>
+      <c r="U18" s="11"/>
     </row>
     <row r="19" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U19" s="11" t="s">
-        <v>613</v>
-      </c>
+      <c r="U19" s="11"/>
     </row>
     <row r="20" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U20" s="11" t="s">
-        <v>614</v>
-      </c>
+      <c r="U20" s="11"/>
     </row>
     <row r="21" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U21" s="11" t="s">
-        <v>601</v>
-      </c>
+      <c r="U21" s="11"/>
     </row>
     <row r="22" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U22" s="11" t="s">
-        <v>615</v>
-      </c>
+      <c r="U22" s="11"/>
     </row>
     <row r="23" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U23" s="11" t="s">
-        <v>610</v>
-      </c>
+      <c r="U23" s="11"/>
     </row>
     <row r="24" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U24" s="11" t="s">
-        <v>616</v>
-      </c>
+      <c r="U24" s="11"/>
     </row>
     <row r="25" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U25" s="11" t="s">
-        <v>601</v>
-      </c>
+      <c r="U25" s="11"/>
     </row>
     <row r="26" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U26" s="11" t="s">
-        <v>612</v>
-      </c>
+      <c r="U26" s="11"/>
     </row>
     <row r="27" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U27" s="11" t="s">
-        <v>617</v>
-      </c>
+      <c r="U27" s="11"/>
     </row>
     <row r="28" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U28" s="10"/>
@@ -2789,142 +2847,34 @@
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U30" s="11" t="s">
-        <v>638</v>
-      </c>
+      <c r="U30" s="11"/>
     </row>
     <row r="31" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U31" s="12" t="s">
-        <v>618</v>
-      </c>
+      <c r="U31" s="12"/>
     </row>
     <row r="32" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U32" s="12" t="s">
-        <v>601</v>
-      </c>
+      <c r="U32" s="12"/>
     </row>
     <row r="33" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U33" s="12" t="s">
-        <v>619</v>
-      </c>
+      <c r="U33" s="12"/>
     </row>
     <row r="34" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U34" s="12" t="s">
-        <v>620</v>
-      </c>
+      <c r="U34" s="12"/>
     </row>
     <row r="35" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U35" s="12"/>
     </row>
     <row r="36" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U36" s="12" t="s">
-        <v>621</v>
-      </c>
+      <c r="U36" s="12"/>
     </row>
     <row r="37" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U37" s="12" t="s">
-        <v>601</v>
-      </c>
+      <c r="U37" s="12"/>
     </row>
     <row r="38" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U38" s="12" t="s">
-        <v>622</v>
-      </c>
+      <c r="U38" s="12"/>
     </row>
     <row r="39" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U39" s="12" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="43" spans="21:21" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="U43" s="14" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="44" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U44" s="13" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="45" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U45" s="13" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="46" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U46" s="13" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="47" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U47" s="13" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="48" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U48" s="13" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="49" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U49" s="13" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="50" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U50" s="13" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="51" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U51" s="13" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="52" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U52" s="13" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="53" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U53" s="13" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="54" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U54" s="13" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="55" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U55" s="13" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="56" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U56" s="13" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="57" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U57" s="13" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="58" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U58" s="13" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="59" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U59" s="13" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="60" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U60" s="13" t="s">
-        <v>635</v>
-      </c>
+      <c r="U39" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2934,6 +2884,456 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:Z11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.90625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>125</v>
+      </c>
+      <c r="B2" s="5">
+        <v>110</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="R2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>126</v>
+      </c>
+      <c r="B3" s="5">
+        <v>110</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="R3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>127</v>
+      </c>
+      <c r="B4" s="5">
+        <v>110</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="R4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>128</v>
+      </c>
+      <c r="B5" s="5">
+        <v>110</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="R5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>129</v>
+      </c>
+      <c r="B6" s="5">
+        <v>110</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="R6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>130</v>
+      </c>
+      <c r="B7" s="5">
+        <v>110</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="R7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>131</v>
+      </c>
+      <c r="B8" s="5">
+        <v>110</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="R8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>133</v>
+      </c>
+      <c r="B9" s="5">
+        <v>110</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="R9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>134</v>
+      </c>
+      <c r="B10" s="5">
+        <v>110</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>174</v>
+      </c>
+      <c r="B11" s="5">
+        <v>110</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="R11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3348,7 +3748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3809,7 +4209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -4192,7 +4592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -4442,7 +4842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -4667,6 +5067,588 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A10:O47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.90625" style="4" customWidth="1"/>
+    <col min="7" max="8" width="10.90625" style="2"/>
+    <col min="9" max="9" width="79.90625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.90625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>624</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>635</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>634</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>622</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>648</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>651</v>
+      </c>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>628</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="50" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>629</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O12" s="17"/>
+    </row>
+    <row r="13" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O13" s="17"/>
+    </row>
+    <row r="14" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>631</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O14" s="17"/>
+    </row>
+    <row r="15" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>632</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O15" s="17"/>
+    </row>
+    <row r="16" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>6</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="50" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>644</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="O17" s="17" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>8</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>646</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>9</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>639</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="39" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>10</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>641</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>11</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>640</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>12</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="50" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>13</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="O23" s="17" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>14</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="O24" s="17" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>15</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="O25" s="17" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H26" s="13"/>
+      <c r="O26" s="17" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H27" s="13"/>
+      <c r="O27" s="17" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H28" s="13"/>
+      <c r="O28" s="17" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H29" s="13"/>
+      <c r="O29" s="17" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H30" s="13"/>
+      <c r="O30" s="17" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H31" s="13"/>
+      <c r="O31" s="17" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H32" s="13"/>
+      <c r="O32" s="17" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="33" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H33" s="13"/>
+      <c r="O33" s="17" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="34" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H34" s="13"/>
+      <c r="O34" s="17" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="35" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H35" s="13"/>
+      <c r="O35" s="17" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H36" s="13"/>
+      <c r="O36" s="12"/>
+    </row>
+    <row r="37" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H37" s="13"/>
+      <c r="O37" s="12"/>
+    </row>
+    <row r="38" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H38" s="13"/>
+      <c r="O38" s="17" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H39" s="13"/>
+      <c r="O39" s="12" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H40" s="13"/>
+      <c r="O40" s="12" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="12" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="12" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O43" s="12"/>
+    </row>
+    <row r="44" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O44" s="12" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="45" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O45" s="12" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O46" s="12" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O47" s="12" t="s">
+        <v>619</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -5769,7 +6751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -6371,7 +7353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -7028,7 +8010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -7415,7 +8397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -7798,7 +8780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -8235,7 +9217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -8811,454 +9793,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:Z11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="10.90625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>125</v>
-      </c>
-      <c r="B2" s="5">
-        <v>110</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>466</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="R2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>126</v>
-      </c>
-      <c r="B3" s="5">
-        <v>110</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="R3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>127</v>
-      </c>
-      <c r="B4" s="5">
-        <v>110</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="R4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>128</v>
-      </c>
-      <c r="B5" s="5">
-        <v>110</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="R5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>129</v>
-      </c>
-      <c r="B6" s="5">
-        <v>110</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="R6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>130</v>
-      </c>
-      <c r="B7" s="5">
-        <v>110</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="R7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>131</v>
-      </c>
-      <c r="B8" s="5">
-        <v>110</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="R8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>133</v>
-      </c>
-      <c r="B9" s="5">
-        <v>110</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="R9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>134</v>
-      </c>
-      <c r="B10" s="5">
-        <v>110</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S10" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>174</v>
-      </c>
-      <c r="B11" s="5">
-        <v>110</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="R11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
xlsx neu gespeichert file korrupt
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="StatusAssetUseItem" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="760">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -2341,6 +2342,21 @@
   </si>
   <si>
     <t>Special scientific interest</t>
+  </si>
+  <si>
+    <t>Wenn das Asset nicht von nationaler Relevanz ist, muss dein Typ definiert werden</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE NOT(IsNatRel): NOT (DEFINED (TypeNatRel));</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE (IsNatRel): DEFINED(TypeNatRel);</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE AssetItemPart-&gt;IsExtract: DEFINED (AssetItemMain);</t>
+  </si>
+  <si>
+    <t>Jedes AssetPart, dass ein Extract ist, muss ein Main besitzen</t>
   </si>
 </sst>
 </file>
@@ -2962,8 +2978,8 @@
   </sheetPr>
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43:U60"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4968,7 +4984,7 @@
   </sheetPr>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -5236,8 +5252,8 @@
   </sheetPr>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5472,10 +5488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:O47"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5491,437 +5507,545 @@
     <col min="10" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+    <row r="1" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>643</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B1" s="18" t="s">
         <v>620</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>631</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>630</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>618</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>619</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>644</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>647</v>
       </c>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>624</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="50" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>625</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>626</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>627</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>628</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>629</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="50" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>640</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>635</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>622</v>
+        <v>634</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>621</v>
+        <v>657</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>624</v>
+        <v>637</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>653</v>
+        <v>645</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>638</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="50" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="26" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>622</v>
+        <v>634</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>648</v>
+        <v>658</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>625</v>
+        <v>636</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="O12" s="17"/>
-    </row>
-    <row r="13" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="H12" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>622</v>
+        <v>634</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>649</v>
+        <v>759</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>626</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>645</v>
+        <v>758</v>
       </c>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:15" ht="26" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>660</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>632</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>622</v>
+        <v>662</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>650</v>
+        <v>661</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>627</v>
+        <v>663</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="O14" s="17" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="50" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>5</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>660</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>632</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>622</v>
+        <v>662</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>628</v>
+        <v>665</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="O15" s="17"/>
-    </row>
-    <row r="16" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+      <c r="H15" s="14"/>
+      <c r="O15" s="17" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>6</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>660</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>632</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>622</v>
+        <v>662</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>652</v>
+        <v>666</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>629</v>
+        <v>667</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>645</v>
       </c>
+      <c r="H16" s="13"/>
       <c r="O16" s="17" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="50" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>7</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>660</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>634</v>
+        <v>662</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>639</v>
+        <v>668</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>640</v>
+        <v>669</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>655</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="H17" s="13"/>
       <c r="O17" s="17" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="25" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>8</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>660</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>634</v>
+        <v>662</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>641</v>
+        <v>755</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>642</v>
+        <v>756</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>654</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="H18" s="13"/>
       <c r="O18" s="17" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="25" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>9</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>660</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>634</v>
+        <v>662</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>656</v>
+        <v>755</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>635</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>638</v>
-      </c>
+        <v>757</v>
+      </c>
+      <c r="H19" s="13"/>
       <c r="O19" s="17" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="39" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>10</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>637</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>638</v>
-      </c>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H20" s="13"/>
       <c r="O20" s="17" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>11</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>636</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>638</v>
-      </c>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H21" s="13"/>
       <c r="O21" s="17" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>12</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>663</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>645</v>
-      </c>
+    <row r="22" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H22" s="13"/>
       <c r="O22" s="17" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="50" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>13</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>664</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>665</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="H23" s="14"/>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H23" s="13"/>
       <c r="O23" s="17" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>14</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>666</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>645</v>
-      </c>
+    <row r="24" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H24" s="13"/>
       <c r="O24" s="17" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>15</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>669</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>645</v>
-      </c>
+        <v>608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H25" s="13"/>
       <c r="O25" s="17" t="s">
         <v>596</v>
@@ -5936,113 +6060,65 @@
     <row r="27" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H27" s="13"/>
       <c r="O27" s="17" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H28" s="13"/>
-      <c r="O28" s="17" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="O28" s="12"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H29" s="13"/>
-      <c r="O29" s="17" t="s">
-        <v>596</v>
-      </c>
+      <c r="O29" s="12"/>
     </row>
     <row r="30" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H30" s="13"/>
       <c r="O30" s="17" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H31" s="13"/>
-      <c r="O31" s="17" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="O31" s="12" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H32" s="13"/>
-      <c r="O32" s="17" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="33" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="H33" s="13"/>
-      <c r="O33" s="17" t="s">
+      <c r="O32" s="12" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="34" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="H34" s="13"/>
-      <c r="O34" s="17" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="35" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="H35" s="13"/>
-      <c r="O35" s="17" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H36" s="13"/>
-      <c r="O36" s="12"/>
-    </row>
-    <row r="37" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H37" s="13"/>
-      <c r="O37" s="12"/>
-    </row>
-    <row r="38" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="H38" s="13"/>
-      <c r="O38" s="17" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H39" s="13"/>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="12" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="12" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="12"/>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="12" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="12" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="12" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O39" s="12" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H40" s="13"/>
-      <c r="O40" s="12" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O41" s="12" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O42" s="12" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O43" s="12"/>
-    </row>
-    <row r="44" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O44" s="12" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="45" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O45" s="12" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O46" s="12" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O47" s="12" t="s">
         <v>615</v>
       </c>
     </row>
@@ -6059,8 +6135,8 @@
   </sheetPr>
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6069,13 +6145,13 @@
     <col min="2" max="2" width="8.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.6328125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="53.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
@@ -7253,7 +7329,7 @@
   </sheetPr>
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -7269,7 +7345,7 @@
     <col min="8" max="8" width="60" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.6328125" style="5" bestFit="1" customWidth="1"/>
@@ -7900,7 +7976,7 @@
   </sheetPr>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -8993,7 +9069,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Xlsx angepasst: Aktuelles UML eingefügt, kleinere Anpassungen im Text
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -29,7 +29,6 @@
     <sheet name="StatusAssetUseItem" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="761">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -2344,9 +2343,6 @@
     <t>Special scientific interest</t>
   </si>
   <si>
-    <t>Wenn das Asset nicht von nationaler Relevanz ist, muss dein Typ definiert werden</t>
-  </si>
-  <si>
     <t>SET CONSTRAINT WHERE NOT(IsNatRel): NOT (DEFINED (TypeNatRel));</t>
   </si>
   <si>
@@ -2357,6 +2353,12 @@
   </si>
   <si>
     <t>Jedes AssetPart, dass ein Extract ist, muss ein Main besitzen</t>
+  </si>
+  <si>
+    <t>Wenn das Asset nicht von nationaler Relevanz ist, darf kein Typ definiert werden</t>
+  </si>
+  <si>
+    <t>Wenn das Asset von nationaler Relevanz ist, muss mindestens ein Typ definiert werden</t>
   </si>
 </sst>
 </file>
@@ -2551,32 +2553,32 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>22408</xdr:colOff>
+      <xdr:colOff>28178</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>44815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>516837</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>394180</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>151776</xdr:rowOff>
+      <xdr:rowOff>89376</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="Gruppieren 5"/>
+        <xdr:cNvPr id="7" name="Gruppieren 6"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5982337" y="208101"/>
-          <a:ext cx="11162429" cy="9994818"/>
-          <a:chOff x="5979863" y="206451"/>
-          <a:chExt cx="11162429" cy="9516507"/>
+          <a:off x="5988107" y="208101"/>
+          <a:ext cx="13320002" cy="9932418"/>
+          <a:chOff x="5988107" y="208101"/>
+          <a:chExt cx="13320002" cy="9932418"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="Grafik 2"/>
+          <xdr:cNvPr id="2" name="Grafik 1"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2589,13 +2591,13 @@
               </a:ext>
             </a:extLst>
           </a:blip>
-          <a:srcRect l="25252" t="13473" r="2184" b="4365"/>
+          <a:srcRect l="23900" t="6539"/>
           <a:stretch/>
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5979863" y="206452"/>
-            <a:ext cx="11162429" cy="9516506"/>
+            <a:off x="6032500" y="317498"/>
+            <a:ext cx="13127079" cy="9783474"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2615,8 +2617,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5985635" y="206451"/>
-            <a:ext cx="11052000" cy="5231457"/>
+            <a:off x="5988109" y="208101"/>
+            <a:ext cx="13320000" cy="4808399"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2666,8 +2668,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5985635" y="5598177"/>
-            <a:ext cx="11052000" cy="4065367"/>
+            <a:off x="5988107" y="5306786"/>
+            <a:ext cx="13320000" cy="4833733"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2979,7 +2981,7 @@
   <dimension ref="A2:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5490,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5850,10 +5852,10 @@
         <v>634</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="O13" s="17"/>
     </row>
@@ -5978,10 +5980,10 @@
         <v>662</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>755</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>756</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>645</v>
@@ -6005,10 +6007,13 @@
         <v>662</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>757</v>
+        <v>756</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>645</v>
       </c>
       <c r="H19" s="13"/>
       <c r="O19" s="17" t="s">
@@ -6135,8 +6140,8 @@
   </sheetPr>
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7329,7 +7334,7 @@
   </sheetPr>
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Obejktkatalog aus UML/INTERLIS-Editor erstellt; xlsx neu gespeichert
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="764">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -2360,6 +2360,18 @@
   <si>
     <t>Wenn das Asset von nationaler Relevanz ist, muss mindestens ein Typ definiert werden</t>
   </si>
+  <si>
+    <t>CONSTRAINTS OF AssetItem =
+  SET CONSTRAINT WHERE IsExtract:
+    DEFINED(\AssetItemMain);
+END;</t>
+  </si>
+  <si>
+    <t>Referenz" auf eine Rolle einer Beziehung gemacht. So \AssetItemMain</t>
+  </si>
+  <si>
+    <t>replaced durch 13</t>
+  </si>
 </sst>
 </file>
 
@@ -2368,7 +2380,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2438,6 +2450,20 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2478,7 +2504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2529,6 +2555,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2980,7 +3018,7 @@
   </sheetPr>
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -5490,10 +5528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5537,25 +5575,25 @@
       <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="23" t="s">
         <v>632</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="23" t="s">
         <v>622</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="25" t="s">
         <v>621</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="26" t="s">
         <v>624</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="23" t="s">
         <v>623</v>
       </c>
       <c r="I2" s="4" t="s">
@@ -5688,25 +5726,25 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="50" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="23" t="s">
         <v>633</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="23" t="s">
         <v>634</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="25" t="s">
         <v>639</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="26" t="s">
         <v>640</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="23" t="s">
         <v>646</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5720,25 +5758,25 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="23" t="s">
         <v>633</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="23" t="s">
         <v>634</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="25" t="s">
         <v>641</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="26" t="s">
         <v>642</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="23" t="s">
         <v>646</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -5839,53 +5877,63 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="23" t="s">
         <v>633</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="23" t="s">
         <v>634</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="25" t="s">
         <v>758</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="26" t="s">
         <v>757</v>
       </c>
+      <c r="G13" s="23" t="s">
+        <v>623</v>
+      </c>
+      <c r="H13" s="2">
+        <v>13</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>763</v>
+      </c>
       <c r="O13" s="17"/>
     </row>
-    <row r="14" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="52" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>660</v>
+      <c r="B14" s="21" t="s">
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>662</v>
+        <v>762</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>661</v>
+        <v>758</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>663</v>
+        <v>761</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="O14" s="17" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="50" x14ac:dyDescent="0.35">
+      <c r="H14" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="O14" s="17"/>
+    </row>
+    <row r="15" spans="1:15" ht="26" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5899,20 +5947,19 @@
         <v>662</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H15" s="14"/>
       <c r="O15" s="17" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="50" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -5926,17 +5973,17 @@
         <v>662</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="14"/>
       <c r="O16" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
@@ -5953,20 +6000,20 @@
         <v>662</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>645</v>
       </c>
       <c r="H17" s="13"/>
       <c r="O17" s="17" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="25" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -5980,17 +6027,17 @@
         <v>662</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>759</v>
+        <v>668</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>755</v>
+        <v>669</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>645</v>
       </c>
       <c r="H18" s="13"/>
       <c r="O18" s="17" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="25" x14ac:dyDescent="0.25">
@@ -6007,123 +6054,150 @@
         <v>662</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>645</v>
       </c>
       <c r="H19" s="13"/>
       <c r="O19" s="17" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>645</v>
+      </c>
       <c r="H20" s="13"/>
       <c r="O20" s="17" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H21" s="13"/>
       <c r="O21" s="17" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H22" s="13"/>
       <c r="O22" s="17" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H23" s="13"/>
       <c r="O23" s="17" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H24" s="13"/>
       <c r="O24" s="17" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H25" s="13"/>
       <c r="O25" s="17" t="s">
-        <v>596</v>
+        <v>608</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H26" s="13"/>
       <c r="O26" s="17" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H27" s="13"/>
       <c r="O27" s="17" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H28" s="13"/>
+      <c r="O28" s="17" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H28" s="13"/>
-      <c r="O28" s="12"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H29" s="13"/>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H30" s="13"/>
-      <c r="O30" s="17" t="s">
+      <c r="O30" s="12"/>
+    </row>
+    <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H31" s="13"/>
+      <c r="O31" s="17" t="s">
         <v>617</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H31" s="13"/>
-      <c r="O31" s="12" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H32" s="13"/>
       <c r="O32" s="12" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="33" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H33" s="13"/>
+      <c r="O33" s="12" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O33" s="12" t="s">
+    <row r="34" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="12" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O34" s="12" t="s">
+    <row r="35" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="12" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O35" s="12"/>
-    </row>
-    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O36" s="12" t="s">
+    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="12"/>
+    </row>
+    <row r="37" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="12" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O37" s="12" t="s">
+    <row r="38" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="12" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O38" s="12" t="s">
+    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="12" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O39" s="12" t="s">
+    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="12" t="s">
         <v>615</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UML, UML-Grafik und xlsx-Doku mit UML aktualisiert
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -2590,33 +2590,33 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28178</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>44815</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>469008</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>78644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>394180</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>89376</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>298180</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>27143</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="7" name="Gruppieren 6"/>
+        <xdr:cNvPr id="9" name="Gruppieren 8"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5988107" y="208101"/>
-          <a:ext cx="13320002" cy="9932418"/>
-          <a:chOff x="5988107" y="208101"/>
-          <a:chExt cx="13320002" cy="9932418"/>
+          <a:off x="5669658" y="78644"/>
+          <a:ext cx="12021172" cy="11207049"/>
+          <a:chOff x="5664463" y="78644"/>
+          <a:chExt cx="12021172" cy="11343863"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="2" name="Grafik 1"/>
+          <xdr:cNvPr id="8" name="Grafik 7"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2629,13 +2629,13 @@
               </a:ext>
             </a:extLst>
           </a:blip>
-          <a:srcRect l="23900" t="6539"/>
+          <a:srcRect l="14982" t="8476" r="8074" b="5025"/>
           <a:stretch/>
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6032500" y="317498"/>
-            <a:ext cx="13127079" cy="9783474"/>
+            <a:off x="5664463" y="78644"/>
+            <a:ext cx="11990107" cy="11343863"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2655,8 +2655,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5988109" y="208101"/>
-            <a:ext cx="13320000" cy="4808399"/>
+            <a:off x="5985635" y="206252"/>
+            <a:ext cx="11700000" cy="5656616"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2706,8 +2706,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5988107" y="5306786"/>
-            <a:ext cx="13320000" cy="4833733"/>
+            <a:off x="5985633" y="6199764"/>
+            <a:ext cx="11700000" cy="5043111"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3018,8 +3018,8 @@
   </sheetPr>
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5530,7 +5530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FormatComposition auf 0..* gesetzt; UML, UML-Grafik und xlsx-Doku mit UML aktualisiert
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -2591,32 +2591,32 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>469008</xdr:colOff>
+      <xdr:colOff>497414</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>78644</xdr:rowOff>
+      <xdr:rowOff>105833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>298180</xdr:colOff>
+      <xdr:colOff>458050</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>27143</xdr:rowOff>
+      <xdr:rowOff>48470</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="9" name="Gruppieren 8"/>
+        <xdr:cNvPr id="3" name="Gruppieren 2"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5669658" y="78644"/>
-          <a:ext cx="12021172" cy="11207049"/>
-          <a:chOff x="5664463" y="78644"/>
-          <a:chExt cx="12021172" cy="11343863"/>
+          <a:off x="5698064" y="105833"/>
+          <a:ext cx="12152636" cy="11201187"/>
+          <a:chOff x="5693831" y="105833"/>
+          <a:chExt cx="12152636" cy="11097470"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="8" name="Grafik 7"/>
+          <xdr:cNvPr id="2" name="Grafik 1"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2629,13 +2629,13 @@
               </a:ext>
             </a:extLst>
           </a:blip>
-          <a:srcRect l="14982" t="8476" r="8074" b="5025"/>
+          <a:srcRect l="15236" t="8715" r="6777" b="5364"/>
           <a:stretch/>
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5664463" y="78644"/>
-            <a:ext cx="11990107" cy="11343863"/>
+            <a:off x="5693831" y="105833"/>
+            <a:ext cx="12152636" cy="11097470"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2655,8 +2655,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5985635" y="206252"/>
-            <a:ext cx="11700000" cy="5656616"/>
+            <a:off x="5986597" y="203546"/>
+            <a:ext cx="11700000" cy="5536675"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2706,8 +2706,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5985633" y="6199764"/>
-            <a:ext cx="11700000" cy="5043111"/>
+            <a:off x="5986595" y="6069974"/>
+            <a:ext cx="11700000" cy="4936179"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3019,7 +3019,7 @@
   <dimension ref="A2:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor error corrected cf. issues #80
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="767">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -2070,12 +2070,6 @@
     <t>SET CONSTRAINT WHERE NOT (InternalUse-&gt;IsAvailable): NOT (PublicUse-&gt;IsAvailable);</t>
   </si>
   <si>
-    <t>Wenn das Startdatum der Öffentichennutzung gesetzt ist, dann muss auch das Startdatum der Internennutzung gesetzt sein und das interne Startdatum muss kleiner oder gleich dem öffentlichen sein</t>
-  </si>
-  <si>
-    <t>SET CONSTRAINT WHERE DEFINED (PublicUse-&gt;DateStartAvailability): DEFINED(InternalUse-&gt;DateStartAvailability) AND (InternalUse-&gt;DateStartAvailability &lt;= PublicUse-&gt;DateStartAvailability);</t>
-  </si>
-  <si>
     <t>Wenn das öffentliche Startdatum gesetzt ist, dann darf der öffentliche Nutzungsstatus nicht auf TRUE (= nutzbar) stehen</t>
   </si>
   <si>
@@ -2371,6 +2365,21 @@
   </si>
   <si>
     <t>replaced durch 13</t>
+  </si>
+  <si>
+    <t>Initially edited</t>
+  </si>
+  <si>
+    <t>Old data imported</t>
+  </si>
+  <si>
+    <t>Wenn das Startdatum der öffentlichen Nutzung gesetzt ist, dann muss entweder der Status der internen Nutzung auf TRUE (= nutzbar) stehen oder (OR) das Startdatum der internen Nutzung gesetzt sein (dann muss der Status der internen Nutzung ja auf FALSE stehen) und (AND) das Startdatum der internen Nutzung muss kleiner oder gleich dem der öffentlichen Nutzung sein.</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE DEFINED (PublicUse-&gt;DateStartAvailability): (InternalUse-&gt;IsAvailable) OR DEFINED(InternalUse-&gt;DateStartAvailability) AND (InternalUse-&gt;DateStartAvailability &lt;= PublicUse-&gt;DateStartAvailability);</t>
+  </si>
+  <si>
+    <t>modified</t>
   </si>
 </sst>
 </file>
@@ -2590,33 +2599,33 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>497414</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>105833</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>208642</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>117927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>458050</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>48470</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>512202</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="Gruppieren 2"/>
+        <xdr:cNvPr id="7" name="Gruppieren 6"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5698064" y="105833"/>
-          <a:ext cx="12152636" cy="11201187"/>
-          <a:chOff x="5693831" y="105833"/>
-          <a:chExt cx="12152636" cy="11097470"/>
+          <a:off x="6168571" y="281213"/>
+          <a:ext cx="10971560" cy="10831286"/>
+          <a:chOff x="6168571" y="281213"/>
+          <a:chExt cx="10971560" cy="10831286"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="2" name="Grafik 1"/>
+          <xdr:cNvPr id="6" name="Grafik 5"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2629,13 +2638,13 @@
               </a:ext>
             </a:extLst>
           </a:blip>
-          <a:srcRect l="15236" t="8715" r="6777" b="5364"/>
+          <a:srcRect l="18421" t="6419" r="5761" b="3478"/>
           <a:stretch/>
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5693831" y="105833"/>
-            <a:ext cx="12152636" cy="11097470"/>
+            <a:off x="6177644" y="281222"/>
+            <a:ext cx="10962487" cy="10822294"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2655,8 +2664,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5986597" y="203546"/>
-            <a:ext cx="11700000" cy="5536675"/>
+            <a:off x="6168573" y="281213"/>
+            <a:ext cx="10912929" cy="5457949"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2706,8 +2715,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5986595" y="6069974"/>
-            <a:ext cx="11700000" cy="4936179"/>
+            <a:off x="6168571" y="6246508"/>
+            <a:ext cx="10912929" cy="4865991"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3018,8 +3027,8 @@
   </sheetPr>
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3336,10 +3345,10 @@
         <v>462</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>58</v>
@@ -3348,7 +3357,7 @@
         <v>461</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -3371,10 +3380,10 @@
         <v>459</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>458</v>
@@ -3383,7 +3392,7 @@
         <v>457</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -3406,10 +3415,10 @@
         <v>455</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>454</v>
@@ -3418,7 +3427,7 @@
         <v>453</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -3441,10 +3450,10 @@
         <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>451</v>
@@ -3453,7 +3462,7 @@
         <v>450</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -3476,10 +3485,10 @@
         <v>448</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>447</v>
@@ -3488,7 +3497,7 @@
         <v>446</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -3511,10 +3520,10 @@
         <v>100</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>99</v>
@@ -3523,7 +3532,7 @@
         <v>98</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -3546,10 +3555,10 @@
         <v>443</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>442</v>
@@ -3558,7 +3567,7 @@
         <v>441</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -3581,10 +3590,10 @@
         <v>439</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>438</v>
@@ -3593,7 +3602,7 @@
         <v>437</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -3616,10 +3625,10 @@
         <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>28</v>
@@ -3628,7 +3637,7 @@
         <v>27</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -3651,10 +3660,10 @@
         <v>434</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>433</v>
@@ -3663,7 +3672,7 @@
         <v>432</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -3831,7 +3840,7 @@
         <v>498</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>498</v>
@@ -3843,7 +3852,7 @@
         <v>496</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -3866,7 +3875,7 @@
         <v>494</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>494</v>
@@ -3878,7 +3887,7 @@
         <v>492</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -3901,7 +3910,7 @@
         <v>490</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>490</v>
@@ -3913,7 +3922,7 @@
         <v>488</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -3936,7 +3945,7 @@
         <v>486</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>486</v>
@@ -3948,7 +3957,7 @@
         <v>484</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -3971,7 +3980,7 @@
         <v>482</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>482</v>
@@ -3983,7 +3992,7 @@
         <v>480</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -4006,7 +4015,7 @@
         <v>478</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>478</v>
@@ -4018,7 +4027,7 @@
         <v>476</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -4041,7 +4050,7 @@
         <v>474</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>474</v>
@@ -4053,7 +4062,7 @@
         <v>472</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -4076,7 +4085,7 @@
         <v>470</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>470</v>
@@ -4088,7 +4097,7 @@
         <v>468</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -4111,7 +4120,7 @@
         <v>466</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>466</v>
@@ -4123,7 +4132,7 @@
         <v>464</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -4288,7 +4297,7 @@
         <v>535</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>535</v>
@@ -4329,7 +4338,7 @@
         <v>532</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>532</v>
@@ -4370,7 +4379,7 @@
         <v>523</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>523</v>
@@ -4411,7 +4420,7 @@
         <v>520</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>520</v>
@@ -4452,7 +4461,7 @@
         <v>517</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>517</v>
@@ -4496,7 +4505,7 @@
         <v>513</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>512</v>
@@ -4540,7 +4549,7 @@
         <v>509</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>509</v>
@@ -4581,7 +4590,7 @@
         <v>502</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>502</v>
@@ -4624,7 +4633,7 @@
   <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4770,10 +4779,10 @@
         <v>568</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>566</v>
+        <v>762</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>567</v>
@@ -4802,7 +4811,7 @@
         <v>564</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>562</v>
@@ -4834,10 +4843,10 @@
         <v>560</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>558</v>
+        <v>763</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>559</v>
@@ -4866,7 +4875,7 @@
         <v>556</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>554</v>
@@ -4898,7 +4907,7 @@
         <v>552</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>550</v>
@@ -4930,7 +4939,7 @@
         <v>548</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>546</v>
@@ -4962,7 +4971,7 @@
         <v>544</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>542</v>
@@ -4994,7 +5003,7 @@
         <v>539</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>539</v>
@@ -5171,7 +5180,7 @@
         <v>583</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>583</v>
@@ -5212,7 +5221,7 @@
         <v>573</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>573</v>
@@ -5253,7 +5262,7 @@
         <v>132</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>132</v>
@@ -5439,7 +5448,7 @@
         <v>594</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>592</v>
@@ -5471,7 +5480,7 @@
         <v>590</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>588</v>
@@ -5503,7 +5512,7 @@
         <v>585</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>585</v>
@@ -5531,7 +5540,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5890,10 +5899,10 @@
         <v>634</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>623</v>
@@ -5902,7 +5911,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="O13" s="17"/>
     </row>
@@ -5917,13 +5926,13 @@
         <v>633</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>645</v>
@@ -5959,7 +5968,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="50" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="100" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -5973,15 +5982,18 @@
         <v>662</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>664</v>
+        <v>764</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>665</v>
+        <v>765</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>645</v>
       </c>
       <c r="H16" s="14"/>
+      <c r="I16" s="4" t="s">
+        <v>766</v>
+      </c>
       <c r="O16" s="17" t="s">
         <v>602</v>
       </c>
@@ -6000,10 +6012,10 @@
         <v>662</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>645</v>
@@ -6027,10 +6039,10 @@
         <v>662</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>645</v>
@@ -6054,10 +6066,10 @@
         <v>662</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>645</v>
@@ -6081,10 +6093,10 @@
         <v>662</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>645</v>
@@ -6339,10 +6351,10 @@
         <v>132</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>131</v>
@@ -6351,7 +6363,7 @@
         <v>130</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -6374,10 +6386,10 @@
         <v>128</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>670</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>672</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>127</v>
@@ -6386,7 +6398,7 @@
         <v>126</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -6409,10 +6421,10 @@
         <v>124</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>123</v>
@@ -6421,7 +6433,7 @@
         <v>122</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -6444,10 +6456,10 @@
         <v>120</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>119</v>
@@ -6456,7 +6468,7 @@
         <v>118</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -6479,10 +6491,10 @@
         <v>115</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>116</v>
@@ -6491,7 +6503,7 @@
         <v>115</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>114</v>
@@ -6517,10 +6529,10 @@
         <v>112</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>111</v>
@@ -6529,7 +6541,7 @@
         <v>110</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -6552,10 +6564,10 @@
         <v>108</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>107</v>
@@ -6564,7 +6576,7 @@
         <v>106</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -6587,10 +6599,10 @@
         <v>104</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>103</v>
@@ -6599,7 +6611,7 @@
         <v>102</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -6622,10 +6634,10 @@
         <v>100</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>99</v>
@@ -6634,7 +6646,7 @@
         <v>98</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -6657,10 +6669,10 @@
         <v>96</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>95</v>
@@ -6669,7 +6681,7 @@
         <v>94</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -6692,7 +6704,7 @@
         <v>92</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>91</v>
@@ -6727,10 +6739,10 @@
         <v>88</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>87</v>
@@ -6739,7 +6751,7 @@
         <v>86</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="R13" s="6" t="b">
         <v>0</v>
@@ -6762,10 +6774,10 @@
         <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>83</v>
@@ -6774,7 +6786,7 @@
         <v>82</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="R14" s="6" t="b">
         <v>0</v>
@@ -6797,10 +6809,10 @@
         <v>80</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>79</v>
@@ -6809,7 +6821,7 @@
         <v>78</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="R15" s="6" t="b">
         <v>0</v>
@@ -6832,10 +6844,10 @@
         <v>76</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>75</v>
@@ -6844,7 +6856,7 @@
         <v>74</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="R16" s="6" t="b">
         <v>0</v>
@@ -6867,10 +6879,10 @@
         <v>72</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>71</v>
@@ -6879,7 +6891,7 @@
         <v>70</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>69</v>
@@ -6905,10 +6917,10 @@
         <v>67</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>66</v>
@@ -6917,7 +6929,7 @@
         <v>65</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="R18" s="6" t="b">
         <v>0</v>
@@ -6940,10 +6952,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>62</v>
@@ -6952,7 +6964,7 @@
         <v>61</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="R19" s="6" t="b">
         <v>0</v>
@@ -6975,10 +6987,10 @@
         <v>59</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>58</v>
@@ -6987,7 +6999,7 @@
         <v>57</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="R20" s="6" t="b">
         <v>0</v>
@@ -7010,10 +7022,10 @@
         <v>55</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>54</v>
@@ -7022,7 +7034,7 @@
         <v>53</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="R21" s="6" t="b">
         <v>0</v>
@@ -7045,10 +7057,10 @@
         <v>51</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>50</v>
@@ -7057,7 +7069,7 @@
         <v>49</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="R22" s="6" t="b">
         <v>0</v>
@@ -7080,7 +7092,7 @@
         <v>46</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>46</v>
@@ -7118,10 +7130,10 @@
         <v>43</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>42</v>
@@ -7130,7 +7142,7 @@
         <v>41</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>40</v>
@@ -7156,7 +7168,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>620</v>
@@ -7194,10 +7206,10 @@
         <v>33</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>32</v>
@@ -7206,7 +7218,7 @@
         <v>31</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>30</v>
@@ -7232,10 +7244,10 @@
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>28</v>
@@ -7244,7 +7256,7 @@
         <v>27</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="R27" s="6" t="b">
         <v>0</v>
@@ -7267,7 +7279,7 @@
         <v>25</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>24</v>
@@ -7302,10 +7314,10 @@
         <v>21</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>20</v>
@@ -7314,7 +7326,7 @@
         <v>19</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="R29" s="6" t="b">
         <v>0</v>
@@ -7337,10 +7349,10 @@
         <v>17</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>16</v>
@@ -7349,7 +7361,7 @@
         <v>15</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>14</v>
@@ -7375,10 +7387,10 @@
         <v>12</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>11</v>
@@ -7387,7 +7399,7 @@
         <v>10</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="R31" s="6" t="b">
         <v>0</v>
@@ -7532,10 +7544,10 @@
         <v>211</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>210</v>
@@ -7544,7 +7556,7 @@
         <v>209</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -7567,10 +7579,10 @@
         <v>207</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>206</v>
@@ -7579,7 +7591,7 @@
         <v>205</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -7602,10 +7614,10 @@
         <v>203</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>202</v>
@@ -7614,7 +7626,7 @@
         <v>201</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -7637,10 +7649,10 @@
         <v>199</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>198</v>
@@ -7649,7 +7661,7 @@
         <v>197</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -7672,10 +7684,10 @@
         <v>195</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>194</v>
@@ -7684,7 +7696,7 @@
         <v>193</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -7707,10 +7719,10 @@
         <v>132</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>191</v>
@@ -7719,7 +7731,7 @@
         <v>130</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -7742,10 +7754,10 @@
         <v>189</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>188</v>
@@ -7754,7 +7766,7 @@
         <v>187</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -7777,10 +7789,10 @@
         <v>185</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>184</v>
@@ -7789,7 +7801,7 @@
         <v>183</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -7812,10 +7824,10 @@
         <v>181</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>180</v>
@@ -7824,7 +7836,7 @@
         <v>179</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -7847,10 +7859,10 @@
         <v>177</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>176</v>
@@ -7859,7 +7871,7 @@
         <v>175</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -7882,10 +7894,10 @@
         <v>173</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>172</v>
@@ -7894,7 +7906,7 @@
         <v>171</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="R12" s="6" t="b">
         <v>0</v>
@@ -7917,10 +7929,10 @@
         <v>169</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>168</v>
@@ -7929,7 +7941,7 @@
         <v>167</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="R13" s="6" t="b">
         <v>0</v>
@@ -7952,10 +7964,10 @@
         <v>165</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>164</v>
@@ -7964,7 +7976,7 @@
         <v>163</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="R14" s="6" t="b">
         <v>0</v>
@@ -7987,7 +7999,7 @@
         <v>160</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>161</v>
@@ -8022,10 +8034,10 @@
         <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>20</v>
@@ -8034,7 +8046,7 @@
         <v>19</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="R16" s="6" t="b">
         <v>0</v>
@@ -8184,10 +8196,10 @@
         <v>132</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>191</v>
@@ -8196,7 +8208,7 @@
         <v>272</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="S2" s="6" t="b">
         <v>0</v>
@@ -8219,10 +8231,10 @@
         <v>270</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>269</v>
@@ -8231,7 +8243,7 @@
         <v>268</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="S3" s="6" t="b">
         <v>0</v>
@@ -8254,10 +8266,10 @@
         <v>266</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>265</v>
@@ -8266,7 +8278,7 @@
         <v>264</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="S4" s="6" t="b">
         <v>0</v>
@@ -8289,10 +8301,10 @@
         <v>262</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>261</v>
@@ -8301,7 +8313,7 @@
         <v>260</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="S5" s="6" t="b">
         <v>0</v>
@@ -8324,10 +8336,10 @@
         <v>258</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>257</v>
@@ -8336,7 +8348,7 @@
         <v>256</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="S6" s="6" t="b">
         <v>0</v>
@@ -8359,10 +8371,10 @@
         <v>254</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>253</v>
@@ -8371,7 +8383,7 @@
         <v>252</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>251</v>
@@ -8397,10 +8409,10 @@
         <v>249</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>248</v>
@@ -8409,7 +8421,7 @@
         <v>247</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>246</v>
@@ -8435,7 +8447,7 @@
         <v>244</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>243</v>
@@ -8470,10 +8482,10 @@
         <v>241</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>240</v>
@@ -8482,7 +8494,7 @@
         <v>239</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="S10" s="6" t="b">
         <v>0</v>
@@ -8505,7 +8517,7 @@
         <v>237</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>236</v>
@@ -8540,7 +8552,7 @@
         <v>234</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>233</v>
@@ -8575,10 +8587,10 @@
         <v>231</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>230</v>
@@ -8587,7 +8599,7 @@
         <v>230</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>229</v>
@@ -8613,10 +8625,10 @@
         <v>21</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>20</v>
@@ -8625,7 +8637,7 @@
         <v>19</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="S14" s="6" t="b">
         <v>0</v>
@@ -8648,7 +8660,7 @@
         <v>226</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>226</v>
@@ -8686,10 +8698,10 @@
         <v>221</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>220</v>
@@ -8698,7 +8710,7 @@
         <v>219</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>218</v>
@@ -8724,10 +8736,10 @@
         <v>216</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>215</v>
@@ -8736,7 +8748,7 @@
         <v>214</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>213</v>
@@ -8862,10 +8874,10 @@
         <v>301</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>298</v>
@@ -8877,7 +8889,7 @@
         <v>299</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>298</v>
@@ -8903,10 +8915,10 @@
         <v>132</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>191</v>
@@ -8918,7 +8930,7 @@
         <v>296</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>191</v>
@@ -8944,10 +8956,10 @@
         <v>291</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>294</v>
@@ -8959,7 +8971,7 @@
         <v>292</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>290</v>
@@ -8985,10 +8997,10 @@
         <v>286</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>285</v>
@@ -9000,7 +9012,7 @@
         <v>287</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>285</v>
@@ -9026,10 +9038,10 @@
         <v>283</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>282</v>
@@ -9041,7 +9053,7 @@
         <v>280</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>279</v>
@@ -9067,7 +9079,7 @@
         <v>277</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>277</v>
@@ -9108,10 +9120,10 @@
         <v>21</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>20</v>
@@ -9123,7 +9135,7 @@
         <v>275</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>20</v>
@@ -9271,7 +9283,7 @@
         <v>346</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>341</v>
@@ -9315,7 +9327,7 @@
         <v>338</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>333</v>
@@ -9359,7 +9371,7 @@
         <v>330</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>325</v>
@@ -9403,7 +9415,7 @@
         <v>322</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>317</v>
@@ -9447,7 +9459,7 @@
         <v>132</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>311</v>
@@ -9491,7 +9503,7 @@
         <v>308</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>304</v>
@@ -9654,10 +9666,10 @@
         <v>387</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>386</v>
@@ -9666,7 +9678,7 @@
         <v>385</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>384</v>
@@ -9692,10 +9704,10 @@
         <v>382</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>381</v>
@@ -9704,7 +9716,7 @@
         <v>380</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>379</v>
@@ -9730,10 +9742,10 @@
         <v>377</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>376</v>
@@ -9742,7 +9754,7 @@
         <v>375</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>374</v>
@@ -9768,10 +9780,10 @@
         <v>372</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>371</v>
@@ -9780,7 +9792,7 @@
         <v>370</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>369</v>
@@ -9806,10 +9818,10 @@
         <v>366</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>367</v>
@@ -9818,7 +9830,7 @@
         <v>366</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>365</v>
@@ -9844,7 +9856,7 @@
         <v>362</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>363</v>
@@ -9882,10 +9894,10 @@
         <v>359</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>358</v>
@@ -9894,7 +9906,7 @@
         <v>357</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>356</v>
@@ -9920,10 +9932,10 @@
         <v>354</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>20</v>
@@ -9932,7 +9944,7 @@
         <v>19</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>353</v>
@@ -9958,10 +9970,10 @@
         <v>351</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>350</v>
@@ -9970,7 +9982,7 @@
         <v>349</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>348</v>
@@ -10141,10 +10153,10 @@
         <v>423</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>422</v>
@@ -10153,7 +10165,7 @@
         <v>421</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -10176,10 +10188,10 @@
         <v>419</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>418</v>
@@ -10188,7 +10200,7 @@
         <v>417</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -10211,10 +10223,10 @@
         <v>415</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>172</v>
@@ -10223,7 +10235,7 @@
         <v>171</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -10246,10 +10258,10 @@
         <v>189</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>188</v>
@@ -10258,7 +10270,7 @@
         <v>187</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -10281,10 +10293,10 @@
         <v>412</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>411</v>
@@ -10293,7 +10305,7 @@
         <v>410</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -10316,10 +10328,10 @@
         <v>408</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>407</v>
@@ -10328,7 +10340,7 @@
         <v>406</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -10351,10 +10363,10 @@
         <v>403</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>404</v>
@@ -10363,7 +10375,7 @@
         <v>403</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -10386,10 +10398,10 @@
         <v>203</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>202</v>
@@ -10398,7 +10410,7 @@
         <v>201</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -10421,10 +10433,10 @@
         <v>177</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>176</v>
@@ -10433,7 +10445,7 @@
         <v>400</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -10456,10 +10468,10 @@
         <v>398</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>397</v>
@@ -10468,7 +10480,7 @@
         <v>209</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -10491,10 +10503,10 @@
         <v>185</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>184</v>
@@ -10503,7 +10515,7 @@
         <v>183</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="R12" s="6" t="b">
         <v>0</v>
@@ -10526,10 +10538,10 @@
         <v>394</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>393</v>
@@ -10538,7 +10550,7 @@
         <v>392</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="R13" s="6" t="b">
         <v>0</v>
@@ -10561,10 +10573,10 @@
         <v>207</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>206</v>
@@ -10573,7 +10585,7 @@
         <v>390</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="R14" s="6" t="b">
         <v>0</v>
@@ -10596,10 +10608,10 @@
         <v>132</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>191</v>
@@ -10608,7 +10620,7 @@
         <v>130</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="R15" s="6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Modified values in StatusWork replaced in xml and xlsx
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="765">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -1714,9 +1714,6 @@
     <t>350778e6-0ebd-4da6-ae9b-8423dcd010df</t>
   </si>
   <si>
-    <t>Imported old</t>
-  </si>
-  <si>
     <t>Importiert Altdaten</t>
   </si>
   <si>
@@ -1736,9 +1733,6 @@
   </si>
   <si>
     <t>751cf7a5-b7b3-4c4c-8804-a18f6a6fde97</t>
-  </si>
-  <si>
-    <t>Initiate Asset</t>
   </si>
   <si>
     <t>Ersterfassung Asset</t>
@@ -3027,7 +3021,7 @@
   </sheetPr>
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
@@ -3345,10 +3339,10 @@
         <v>462</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>58</v>
@@ -3357,7 +3351,7 @@
         <v>461</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -3380,10 +3374,10 @@
         <v>459</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>458</v>
@@ -3392,7 +3386,7 @@
         <v>457</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -3415,10 +3409,10 @@
         <v>455</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>454</v>
@@ -3427,7 +3421,7 @@
         <v>453</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -3450,10 +3444,10 @@
         <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>451</v>
@@ -3462,7 +3456,7 @@
         <v>450</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -3485,10 +3479,10 @@
         <v>448</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>447</v>
@@ -3497,7 +3491,7 @@
         <v>446</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -3520,10 +3514,10 @@
         <v>100</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>99</v>
@@ -3532,7 +3526,7 @@
         <v>98</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -3555,10 +3549,10 @@
         <v>443</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>442</v>
@@ -3567,7 +3561,7 @@
         <v>441</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -3590,10 +3584,10 @@
         <v>439</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>438</v>
@@ -3602,7 +3596,7 @@
         <v>437</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -3625,10 +3619,10 @@
         <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>28</v>
@@ -3637,7 +3631,7 @@
         <v>27</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -3660,10 +3654,10 @@
         <v>434</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>433</v>
@@ -3672,7 +3666,7 @@
         <v>432</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -3840,7 +3834,7 @@
         <v>498</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>498</v>
@@ -3852,7 +3846,7 @@
         <v>496</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -3875,7 +3869,7 @@
         <v>494</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>494</v>
@@ -3887,7 +3881,7 @@
         <v>492</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -3910,7 +3904,7 @@
         <v>490</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>490</v>
@@ -3922,7 +3916,7 @@
         <v>488</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -3945,7 +3939,7 @@
         <v>486</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>486</v>
@@ -3957,7 +3951,7 @@
         <v>484</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -3980,7 +3974,7 @@
         <v>482</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>482</v>
@@ -3992,7 +3986,7 @@
         <v>480</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -4015,7 +4009,7 @@
         <v>478</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>478</v>
@@ -4027,7 +4021,7 @@
         <v>476</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -4050,7 +4044,7 @@
         <v>474</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>474</v>
@@ -4062,7 +4056,7 @@
         <v>472</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -4085,7 +4079,7 @@
         <v>470</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>470</v>
@@ -4097,7 +4091,7 @@
         <v>468</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -4120,7 +4114,7 @@
         <v>466</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>466</v>
@@ -4132,7 +4126,7 @@
         <v>464</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -4297,7 +4291,7 @@
         <v>535</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>535</v>
@@ -4338,7 +4332,7 @@
         <v>532</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>532</v>
@@ -4379,7 +4373,7 @@
         <v>523</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>523</v>
@@ -4420,7 +4414,7 @@
         <v>520</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>520</v>
@@ -4461,7 +4455,7 @@
         <v>517</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>517</v>
@@ -4505,7 +4499,7 @@
         <v>513</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>512</v>
@@ -4549,7 +4543,7 @@
         <v>509</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>509</v>
@@ -4590,7 +4584,7 @@
         <v>502</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>502</v>
@@ -4632,8 +4626,8 @@
   </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4773,22 +4767,22 @@
         <v>112</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>566</v>
+        <v>760</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -4805,22 +4799,22 @@
         <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>563</v>
-      </c>
       <c r="K3" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -4837,22 +4831,22 @@
         <v>112</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>558</v>
+        <v>761</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -4875,7 +4869,7 @@
         <v>556</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>554</v>
@@ -4907,7 +4901,7 @@
         <v>552</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>550</v>
@@ -4939,7 +4933,7 @@
         <v>548</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>546</v>
@@ -4971,7 +4965,7 @@
         <v>544</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>542</v>
@@ -5003,7 +4997,7 @@
         <v>539</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>539</v>
@@ -5174,31 +5168,31 @@
         <v>112</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -5215,31 +5209,31 @@
         <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>668</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>575</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -5256,13 +5250,13 @@
         <v>112</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>132</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>132</v>
@@ -5280,7 +5274,7 @@
         <v>132</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -5442,22 +5436,22 @@
         <v>112</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -5474,22 +5468,22 @@
         <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -5506,22 +5500,22 @@
         <v>112</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -5558,28 +5552,28 @@
   <sheetData>
     <row r="1" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="I1" s="19"/>
     </row>
@@ -5591,25 +5585,25 @@
         <v>7</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>620</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>619</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>622</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="G2" s="23" t="s">
         <v>621</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>624</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>623</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="50" x14ac:dyDescent="0.25">
@@ -5620,19 +5614,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O3" s="17"/>
     </row>
@@ -5644,19 +5638,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O4" s="17"/>
     </row>
@@ -5668,19 +5662,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O5" s="17"/>
     </row>
@@ -5692,19 +5686,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O6" s="17"/>
     </row>
@@ -5716,22 +5710,22 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="50" x14ac:dyDescent="0.25">
@@ -5742,28 +5736,28 @@
         <v>7</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="26" x14ac:dyDescent="0.25">
@@ -5774,28 +5768,28 @@
         <v>7</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="62.5" x14ac:dyDescent="0.25">
@@ -5806,25 +5800,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>635</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="O10" s="17" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="39" x14ac:dyDescent="0.25">
@@ -5835,25 +5829,25 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="26" x14ac:dyDescent="0.25">
@@ -5864,25 +5858,25 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>634</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>638</v>
-      </c>
       <c r="O12" s="17" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="25" x14ac:dyDescent="0.25">
@@ -5893,25 +5887,25 @@
         <v>7</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H13" s="2">
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="O13" s="17"/>
     </row>
@@ -5923,22 +5917,22 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="O14" s="17"/>
     </row>
@@ -5947,25 +5941,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="E15" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>661</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>663</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="100" x14ac:dyDescent="0.35">
@@ -5973,29 +5967,29 @@
         <v>15</v>
       </c>
       <c r="B16" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="4" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
@@ -6003,26 +5997,26 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>664</v>
-      </c>
       <c r="F17" s="20" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H17" s="13"/>
       <c r="O17" s="17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
@@ -6030,26 +6024,26 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H18" s="13"/>
       <c r="O18" s="17" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="25" x14ac:dyDescent="0.25">
@@ -6057,26 +6051,26 @@
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="E19" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H19" s="13"/>
       <c r="O19" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="25" x14ac:dyDescent="0.25">
@@ -6084,74 +6078,74 @@
         <v>19</v>
       </c>
       <c r="B20" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>662</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H20" s="13"/>
       <c r="O20" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H21" s="13"/>
       <c r="O21" s="17" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H22" s="13"/>
       <c r="O22" s="17" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H23" s="13"/>
       <c r="O23" s="17" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H24" s="13"/>
       <c r="O24" s="17" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H25" s="13"/>
       <c r="O25" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H26" s="13"/>
       <c r="O26" s="17" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H27" s="13"/>
       <c r="O27" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H28" s="13"/>
       <c r="O28" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -6165,29 +6159,29 @@
     <row r="31" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H31" s="13"/>
       <c r="O31" s="17" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H32" s="13"/>
       <c r="O32" s="12" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="33" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H33" s="13"/>
       <c r="O33" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O34" s="12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="35" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O35" s="12" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="36" spans="8:15" x14ac:dyDescent="0.25">
@@ -6195,22 +6189,22 @@
     </row>
     <row r="37" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O37" s="12" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="38" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O38" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="39" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O39" s="12" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="40" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O40" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -6351,10 +6345,10 @@
         <v>132</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>131</v>
@@ -6363,7 +6357,7 @@
         <v>130</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -6386,10 +6380,10 @@
         <v>128</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>668</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>670</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>127</v>
@@ -6398,7 +6392,7 @@
         <v>126</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -6421,10 +6415,10 @@
         <v>124</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>123</v>
@@ -6433,7 +6427,7 @@
         <v>122</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -6456,10 +6450,10 @@
         <v>120</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>119</v>
@@ -6468,7 +6462,7 @@
         <v>118</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -6491,10 +6485,10 @@
         <v>115</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>116</v>
@@ -6503,7 +6497,7 @@
         <v>115</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>114</v>
@@ -6529,10 +6523,10 @@
         <v>112</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>111</v>
@@ -6541,7 +6535,7 @@
         <v>110</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -6564,10 +6558,10 @@
         <v>108</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>107</v>
@@ -6576,7 +6570,7 @@
         <v>106</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -6599,10 +6593,10 @@
         <v>104</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>103</v>
@@ -6611,7 +6605,7 @@
         <v>102</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -6634,10 +6628,10 @@
         <v>100</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>99</v>
@@ -6646,7 +6640,7 @@
         <v>98</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -6669,10 +6663,10 @@
         <v>96</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>95</v>
@@ -6681,7 +6675,7 @@
         <v>94</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -6704,7 +6698,7 @@
         <v>92</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>91</v>
@@ -6739,10 +6733,10 @@
         <v>88</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>87</v>
@@ -6751,7 +6745,7 @@
         <v>86</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="R13" s="6" t="b">
         <v>0</v>
@@ -6774,10 +6768,10 @@
         <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>83</v>
@@ -6786,7 +6780,7 @@
         <v>82</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="R14" s="6" t="b">
         <v>0</v>
@@ -6809,10 +6803,10 @@
         <v>80</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>79</v>
@@ -6821,7 +6815,7 @@
         <v>78</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="R15" s="6" t="b">
         <v>0</v>
@@ -6844,10 +6838,10 @@
         <v>76</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>75</v>
@@ -6856,7 +6850,7 @@
         <v>74</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="R16" s="6" t="b">
         <v>0</v>
@@ -6879,10 +6873,10 @@
         <v>72</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>71</v>
@@ -6891,7 +6885,7 @@
         <v>70</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>69</v>
@@ -6917,10 +6911,10 @@
         <v>67</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>66</v>
@@ -6929,7 +6923,7 @@
         <v>65</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="R18" s="6" t="b">
         <v>0</v>
@@ -6952,10 +6946,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>62</v>
@@ -6964,7 +6958,7 @@
         <v>61</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="R19" s="6" t="b">
         <v>0</v>
@@ -6987,10 +6981,10 @@
         <v>59</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>58</v>
@@ -6999,7 +6993,7 @@
         <v>57</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="R20" s="6" t="b">
         <v>0</v>
@@ -7022,10 +7016,10 @@
         <v>55</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>54</v>
@@ -7034,7 +7028,7 @@
         <v>53</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="R21" s="6" t="b">
         <v>0</v>
@@ -7057,10 +7051,10 @@
         <v>51</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>50</v>
@@ -7069,7 +7063,7 @@
         <v>49</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="R22" s="6" t="b">
         <v>0</v>
@@ -7092,7 +7086,7 @@
         <v>46</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>46</v>
@@ -7130,10 +7124,10 @@
         <v>43</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>42</v>
@@ -7142,7 +7136,7 @@
         <v>41</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>40</v>
@@ -7168,10 +7162,10 @@
         <v>38</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>37</v>
@@ -7180,7 +7174,7 @@
         <v>36</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>35</v>
@@ -7206,10 +7200,10 @@
         <v>33</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>32</v>
@@ -7218,7 +7212,7 @@
         <v>31</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>30</v>
@@ -7244,10 +7238,10 @@
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>28</v>
@@ -7256,7 +7250,7 @@
         <v>27</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="R27" s="6" t="b">
         <v>0</v>
@@ -7279,7 +7273,7 @@
         <v>25</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>24</v>
@@ -7314,10 +7308,10 @@
         <v>21</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>20</v>
@@ -7326,7 +7320,7 @@
         <v>19</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="R29" s="6" t="b">
         <v>0</v>
@@ -7349,10 +7343,10 @@
         <v>17</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>16</v>
@@ -7361,7 +7355,7 @@
         <v>15</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>14</v>
@@ -7387,10 +7381,10 @@
         <v>12</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>11</v>
@@ -7399,7 +7393,7 @@
         <v>10</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="R31" s="6" t="b">
         <v>0</v>
@@ -7544,10 +7538,10 @@
         <v>211</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>210</v>
@@ -7556,7 +7550,7 @@
         <v>209</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -7579,10 +7573,10 @@
         <v>207</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>206</v>
@@ -7591,7 +7585,7 @@
         <v>205</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -7614,10 +7608,10 @@
         <v>203</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>202</v>
@@ -7626,7 +7620,7 @@
         <v>201</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -7649,10 +7643,10 @@
         <v>199</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>198</v>
@@ -7661,7 +7655,7 @@
         <v>197</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -7684,10 +7678,10 @@
         <v>195</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>194</v>
@@ -7696,7 +7690,7 @@
         <v>193</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -7719,10 +7713,10 @@
         <v>132</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>191</v>
@@ -7731,7 +7725,7 @@
         <v>130</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -7754,10 +7748,10 @@
         <v>189</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>188</v>
@@ -7766,7 +7760,7 @@
         <v>187</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -7789,10 +7783,10 @@
         <v>185</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>184</v>
@@ -7801,7 +7795,7 @@
         <v>183</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -7824,10 +7818,10 @@
         <v>181</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>180</v>
@@ -7836,7 +7830,7 @@
         <v>179</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -7859,10 +7853,10 @@
         <v>177</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>176</v>
@@ -7871,7 +7865,7 @@
         <v>175</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -7894,10 +7888,10 @@
         <v>173</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>172</v>
@@ -7906,7 +7900,7 @@
         <v>171</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="R12" s="6" t="b">
         <v>0</v>
@@ -7929,10 +7923,10 @@
         <v>169</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>168</v>
@@ -7941,7 +7935,7 @@
         <v>167</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="R13" s="6" t="b">
         <v>0</v>
@@ -7964,10 +7958,10 @@
         <v>165</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>164</v>
@@ -7976,7 +7970,7 @@
         <v>163</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="R14" s="6" t="b">
         <v>0</v>
@@ -7999,7 +7993,7 @@
         <v>160</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>161</v>
@@ -8034,10 +8028,10 @@
         <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>20</v>
@@ -8046,7 +8040,7 @@
         <v>19</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="R16" s="6" t="b">
         <v>0</v>
@@ -8196,10 +8190,10 @@
         <v>132</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>191</v>
@@ -8208,7 +8202,7 @@
         <v>272</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="S2" s="6" t="b">
         <v>0</v>
@@ -8231,10 +8225,10 @@
         <v>270</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>269</v>
@@ -8243,7 +8237,7 @@
         <v>268</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="S3" s="6" t="b">
         <v>0</v>
@@ -8266,10 +8260,10 @@
         <v>266</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>265</v>
@@ -8278,7 +8272,7 @@
         <v>264</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="S4" s="6" t="b">
         <v>0</v>
@@ -8301,10 +8295,10 @@
         <v>262</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>261</v>
@@ -8313,7 +8307,7 @@
         <v>260</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="S5" s="6" t="b">
         <v>0</v>
@@ -8336,10 +8330,10 @@
         <v>258</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>257</v>
@@ -8348,7 +8342,7 @@
         <v>256</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="S6" s="6" t="b">
         <v>0</v>
@@ -8371,10 +8365,10 @@
         <v>254</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>253</v>
@@ -8383,7 +8377,7 @@
         <v>252</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>251</v>
@@ -8409,10 +8403,10 @@
         <v>249</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>248</v>
@@ -8421,7 +8415,7 @@
         <v>247</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>246</v>
@@ -8447,7 +8441,7 @@
         <v>244</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>243</v>
@@ -8482,10 +8476,10 @@
         <v>241</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>240</v>
@@ -8494,7 +8488,7 @@
         <v>239</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="S10" s="6" t="b">
         <v>0</v>
@@ -8517,7 +8511,7 @@
         <v>237</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>236</v>
@@ -8552,7 +8546,7 @@
         <v>234</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>233</v>
@@ -8587,10 +8581,10 @@
         <v>231</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>230</v>
@@ -8599,7 +8593,7 @@
         <v>230</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>229</v>
@@ -8625,10 +8619,10 @@
         <v>21</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>20</v>
@@ -8637,7 +8631,7 @@
         <v>19</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="S14" s="6" t="b">
         <v>0</v>
@@ -8660,7 +8654,7 @@
         <v>226</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>226</v>
@@ -8698,10 +8692,10 @@
         <v>221</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>220</v>
@@ -8710,7 +8704,7 @@
         <v>219</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>218</v>
@@ -8736,10 +8730,10 @@
         <v>216</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>215</v>
@@ -8748,7 +8742,7 @@
         <v>214</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>213</v>
@@ -8874,10 +8868,10 @@
         <v>301</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>298</v>
@@ -8889,7 +8883,7 @@
         <v>299</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>298</v>
@@ -8915,10 +8909,10 @@
         <v>132</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>191</v>
@@ -8930,7 +8924,7 @@
         <v>296</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>191</v>
@@ -8956,10 +8950,10 @@
         <v>291</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>294</v>
@@ -8971,7 +8965,7 @@
         <v>292</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>290</v>
@@ -8997,10 +8991,10 @@
         <v>286</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>285</v>
@@ -9012,7 +9006,7 @@
         <v>287</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>285</v>
@@ -9038,10 +9032,10 @@
         <v>283</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>282</v>
@@ -9053,7 +9047,7 @@
         <v>280</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>279</v>
@@ -9079,7 +9073,7 @@
         <v>277</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>277</v>
@@ -9120,10 +9114,10 @@
         <v>21</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>20</v>
@@ -9135,7 +9129,7 @@
         <v>275</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>20</v>
@@ -9283,7 +9277,7 @@
         <v>346</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>341</v>
@@ -9327,7 +9321,7 @@
         <v>338</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>333</v>
@@ -9371,7 +9365,7 @@
         <v>330</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>325</v>
@@ -9415,7 +9409,7 @@
         <v>322</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>317</v>
@@ -9459,7 +9453,7 @@
         <v>132</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>311</v>
@@ -9503,7 +9497,7 @@
         <v>308</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>304</v>
@@ -9666,10 +9660,10 @@
         <v>387</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>386</v>
@@ -9678,7 +9672,7 @@
         <v>385</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>384</v>
@@ -9704,10 +9698,10 @@
         <v>382</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>381</v>
@@ -9716,7 +9710,7 @@
         <v>380</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>379</v>
@@ -9742,10 +9736,10 @@
         <v>377</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>376</v>
@@ -9754,7 +9748,7 @@
         <v>375</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>374</v>
@@ -9780,10 +9774,10 @@
         <v>372</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>371</v>
@@ -9792,7 +9786,7 @@
         <v>370</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>369</v>
@@ -9818,10 +9812,10 @@
         <v>366</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>367</v>
@@ -9830,7 +9824,7 @@
         <v>366</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>365</v>
@@ -9856,7 +9850,7 @@
         <v>362</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>363</v>
@@ -9894,10 +9888,10 @@
         <v>359</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>358</v>
@@ -9906,7 +9900,7 @@
         <v>357</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>356</v>
@@ -9932,10 +9926,10 @@
         <v>354</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>20</v>
@@ -9944,7 +9938,7 @@
         <v>19</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>353</v>
@@ -9970,10 +9964,10 @@
         <v>351</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>350</v>
@@ -9982,7 +9976,7 @@
         <v>349</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>348</v>
@@ -10153,10 +10147,10 @@
         <v>423</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>422</v>
@@ -10165,7 +10159,7 @@
         <v>421</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="R2" s="6" t="b">
         <v>0</v>
@@ -10188,10 +10182,10 @@
         <v>419</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>418</v>
@@ -10200,7 +10194,7 @@
         <v>417</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="R3" s="6" t="b">
         <v>0</v>
@@ -10223,10 +10217,10 @@
         <v>415</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>172</v>
@@ -10235,7 +10229,7 @@
         <v>171</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="R4" s="6" t="b">
         <v>0</v>
@@ -10258,10 +10252,10 @@
         <v>189</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>188</v>
@@ -10270,7 +10264,7 @@
         <v>187</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="R5" s="6" t="b">
         <v>0</v>
@@ -10293,10 +10287,10 @@
         <v>412</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>411</v>
@@ -10305,7 +10299,7 @@
         <v>410</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="R6" s="6" t="b">
         <v>0</v>
@@ -10328,10 +10322,10 @@
         <v>408</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>407</v>
@@ -10340,7 +10334,7 @@
         <v>406</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="R7" s="6" t="b">
         <v>0</v>
@@ -10363,10 +10357,10 @@
         <v>403</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>404</v>
@@ -10375,7 +10369,7 @@
         <v>403</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="R8" s="6" t="b">
         <v>0</v>
@@ -10398,10 +10392,10 @@
         <v>203</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>202</v>
@@ -10410,7 +10404,7 @@
         <v>201</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="R9" s="6" t="b">
         <v>0</v>
@@ -10433,10 +10427,10 @@
         <v>177</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>176</v>
@@ -10445,7 +10439,7 @@
         <v>400</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="R10" s="6" t="b">
         <v>0</v>
@@ -10468,10 +10462,10 @@
         <v>398</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>397</v>
@@ -10480,7 +10474,7 @@
         <v>209</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="R11" s="6" t="b">
         <v>0</v>
@@ -10503,10 +10497,10 @@
         <v>185</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>184</v>
@@ -10515,7 +10509,7 @@
         <v>183</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="R12" s="6" t="b">
         <v>0</v>
@@ -10538,10 +10532,10 @@
         <v>394</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>393</v>
@@ -10550,7 +10544,7 @@
         <v>392</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="R13" s="6" t="b">
         <v>0</v>
@@ -10573,10 +10567,10 @@
         <v>207</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>206</v>
@@ -10585,7 +10579,7 @@
         <v>390</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="R14" s="6" t="b">
         <v>0</v>
@@ -10608,10 +10602,10 @@
         <v>132</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>191</v>
@@ -10620,7 +10614,7 @@
         <v>130</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="R15" s="6" t="b">
         <v>0</v>

</xml_diff>